<commit_message>
Updated cleaning, added shannon and permanova calcs
</commit_message>
<xml_diff>
--- a/R/2017_07_27_Completed_LW1_deep (-5m to 95m)_newcleaned.xlsx
+++ b/R/2017_07_27_Completed_LW1_deep (-5m to 95m)_newcleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yeozy\Documents\Yale-NUS\Y3S1\UROPS\UROPS\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{21FD98C5-C0C9-4CBF-83ED-29A8B5B3F552}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{32DB31A7-BD8A-42FA-8F9A-0FFE18F5E926}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="753" yWindow="222" windowWidth="17191" windowHeight="15220" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8839,11 +8839,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T370"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A345" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P153" sqref="P153"/>
     </sheetView>
   </sheetViews>
@@ -8919,7 +8918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1">
+    <row r="2" spans="1:20">
       <c r="A2" s="19">
         <v>42937</v>
       </c>
@@ -8946,7 +8945,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="3" spans="1:20" hidden="1">
+    <row r="3" spans="1:20">
       <c r="A3" s="19">
         <v>42937</v>
       </c>
@@ -8973,7 +8972,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="4" spans="1:20" hidden="1">
+    <row r="4" spans="1:20">
       <c r="A4" s="19">
         <v>42937</v>
       </c>
@@ -9039,7 +9038,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="6" spans="1:20" hidden="1">
+    <row r="6" spans="1:20">
       <c r="A6" s="19">
         <v>42937</v>
       </c>
@@ -9066,7 +9065,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="7" spans="1:20" hidden="1">
+    <row r="7" spans="1:20">
       <c r="A7" s="19">
         <v>42937</v>
       </c>
@@ -9093,7 +9092,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:20" hidden="1">
+    <row r="8" spans="1:20">
       <c r="A8" s="19">
         <v>42937</v>
       </c>
@@ -9159,7 +9158,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="10" spans="1:20" hidden="1">
+    <row r="10" spans="1:20">
       <c r="A10" s="19">
         <v>42937</v>
       </c>
@@ -9186,7 +9185,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="11" spans="1:20" hidden="1">
+    <row r="11" spans="1:20">
       <c r="A11" s="19">
         <v>42937</v>
       </c>
@@ -9213,7 +9212,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:20" hidden="1">
+    <row r="12" spans="1:20">
       <c r="A12" s="19">
         <v>42937</v>
       </c>
@@ -9279,7 +9278,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="14" spans="1:20" hidden="1">
+    <row r="14" spans="1:20">
       <c r="A14" s="19">
         <v>42937</v>
       </c>
@@ -9306,7 +9305,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1">
+    <row r="15" spans="1:20">
       <c r="A15" s="19">
         <v>42937</v>
       </c>
@@ -9333,7 +9332,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:20" hidden="1">
+    <row r="16" spans="1:20">
       <c r="A16" s="19">
         <v>42937</v>
       </c>
@@ -9360,7 +9359,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1">
+    <row r="17" spans="1:13">
       <c r="A17" s="19">
         <v>42937</v>
       </c>
@@ -9387,7 +9386,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1">
+    <row r="18" spans="1:13">
       <c r="A18" s="19">
         <v>42937</v>
       </c>
@@ -9414,7 +9413,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1">
+    <row r="19" spans="1:13">
       <c r="A19" s="19">
         <v>42937</v>
       </c>
@@ -9441,7 +9440,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1">
+    <row r="20" spans="1:13">
       <c r="A20" s="19">
         <v>42937</v>
       </c>
@@ -9507,7 +9506,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1">
+    <row r="22" spans="1:13">
       <c r="A22" s="19">
         <v>42937</v>
       </c>
@@ -9573,7 +9572,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1">
+    <row r="24" spans="1:13">
       <c r="A24" s="19">
         <v>42937</v>
       </c>
@@ -9639,7 +9638,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1">
+    <row r="26" spans="1:13">
       <c r="A26" s="19">
         <v>42937</v>
       </c>
@@ -9666,7 +9665,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1">
+    <row r="27" spans="1:13">
       <c r="A27" s="19">
         <v>42937</v>
       </c>
@@ -9693,7 +9692,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1">
+    <row r="28" spans="1:13">
       <c r="A28" s="19">
         <v>42937</v>
       </c>
@@ -9759,7 +9758,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1">
+    <row r="30" spans="1:13">
       <c r="A30" s="19">
         <v>42937</v>
       </c>
@@ -9786,7 +9785,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1">
+    <row r="31" spans="1:13">
       <c r="A31" s="19">
         <v>42937</v>
       </c>
@@ -9813,7 +9812,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1">
+    <row r="32" spans="1:13">
       <c r="A32" s="19">
         <v>42937</v>
       </c>
@@ -9879,7 +9878,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1">
+    <row r="34" spans="1:13">
       <c r="A34" s="19">
         <v>42937</v>
       </c>
@@ -9906,7 +9905,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1">
+    <row r="35" spans="1:13">
       <c r="A35" s="19">
         <v>42937</v>
       </c>
@@ -9933,7 +9932,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1">
+    <row r="36" spans="1:13">
       <c r="A36" s="19">
         <v>42937</v>
       </c>
@@ -9999,7 +9998,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1">
+    <row r="38" spans="1:13">
       <c r="A38" s="19">
         <v>42937</v>
       </c>
@@ -10029,7 +10028,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1">
+    <row r="39" spans="1:13">
       <c r="A39" s="19">
         <v>42937</v>
       </c>
@@ -10056,7 +10055,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1">
+    <row r="40" spans="1:13">
       <c r="A40" s="19">
         <v>42937</v>
       </c>
@@ -10086,7 +10085,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1">
+    <row r="41" spans="1:13">
       <c r="A41" s="19">
         <v>42937</v>
       </c>
@@ -10151,7 +10150,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1">
+    <row r="43" spans="1:13">
       <c r="A43" s="19">
         <v>42937</v>
       </c>
@@ -10224,7 +10223,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1">
+    <row r="45" spans="1:13">
       <c r="A45" s="19">
         <v>42937</v>
       </c>
@@ -10255,7 +10254,7 @@
       <c r="K45" s="23"/>
       <c r="L45" s="23"/>
     </row>
-    <row r="46" spans="1:13" hidden="1">
+    <row r="46" spans="1:13">
       <c r="A46" s="19">
         <v>42937</v>
       </c>
@@ -10286,7 +10285,7 @@
       <c r="K46" s="23"/>
       <c r="L46" s="23"/>
     </row>
-    <row r="47" spans="1:13" hidden="1">
+    <row r="47" spans="1:13">
       <c r="A47" s="19">
         <v>42937</v>
       </c>
@@ -10317,7 +10316,7 @@
       <c r="K47" s="23"/>
       <c r="L47" s="23"/>
     </row>
-    <row r="48" spans="1:13" hidden="1">
+    <row r="48" spans="1:13">
       <c r="A48" s="19">
         <v>42937</v>
       </c>
@@ -10348,7 +10347,7 @@
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
     </row>
-    <row r="49" spans="1:13" hidden="1">
+    <row r="49" spans="1:13">
       <c r="A49" s="19">
         <v>42937</v>
       </c>
@@ -10379,7 +10378,7 @@
       <c r="K49" s="23"/>
       <c r="L49" s="23"/>
     </row>
-    <row r="50" spans="1:13" hidden="1">
+    <row r="50" spans="1:13">
       <c r="A50" s="19">
         <v>42937</v>
       </c>
@@ -10452,7 +10451,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1">
+    <row r="52" spans="1:13">
       <c r="A52" s="19">
         <v>42937</v>
       </c>
@@ -10483,7 +10482,7 @@
       <c r="K52" s="23"/>
       <c r="L52" s="23"/>
     </row>
-    <row r="53" spans="1:13" hidden="1">
+    <row r="53" spans="1:13">
       <c r="A53" s="19">
         <v>42937</v>
       </c>
@@ -10515,7 +10514,7 @@
       <c r="J53" s="22"/>
       <c r="L53" s="23"/>
     </row>
-    <row r="54" spans="1:13" hidden="1">
+    <row r="54" spans="1:13">
       <c r="A54" s="19">
         <v>42937</v>
       </c>
@@ -10588,7 +10587,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1">
+    <row r="56" spans="1:13">
       <c r="A56" s="19">
         <v>42937</v>
       </c>
@@ -10658,7 +10657,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="58" spans="1:13" hidden="1">
+    <row r="58" spans="1:13">
       <c r="A58" s="19">
         <v>42937</v>
       </c>
@@ -10689,7 +10688,7 @@
       <c r="K58" s="23"/>
       <c r="L58" s="23"/>
     </row>
-    <row r="59" spans="1:13" hidden="1">
+    <row r="59" spans="1:13">
       <c r="A59" s="19">
         <v>42937</v>
       </c>
@@ -10720,7 +10719,7 @@
       <c r="K59" s="23"/>
       <c r="L59" s="23"/>
     </row>
-    <row r="60" spans="1:13" hidden="1">
+    <row r="60" spans="1:13">
       <c r="A60" s="19">
         <v>42937</v>
       </c>
@@ -10751,7 +10750,7 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
     </row>
-    <row r="61" spans="1:13" hidden="1">
+    <row r="61" spans="1:13">
       <c r="A61" s="19">
         <v>42937</v>
       </c>
@@ -10782,7 +10781,7 @@
       <c r="K61" s="23"/>
       <c r="L61" s="23"/>
     </row>
-    <row r="62" spans="1:13" hidden="1">
+    <row r="62" spans="1:13">
       <c r="A62" s="19">
         <v>42937</v>
       </c>
@@ -10813,7 +10812,7 @@
       <c r="K62" s="23"/>
       <c r="L62" s="23"/>
     </row>
-    <row r="63" spans="1:13" hidden="1">
+    <row r="63" spans="1:13">
       <c r="A63" s="19">
         <v>42937</v>
       </c>
@@ -10844,7 +10843,7 @@
       <c r="K63" s="23"/>
       <c r="L63" s="23"/>
     </row>
-    <row r="64" spans="1:13" hidden="1">
+    <row r="64" spans="1:13">
       <c r="A64" s="19">
         <v>42937</v>
       </c>
@@ -10875,7 +10874,7 @@
       <c r="K64" s="23"/>
       <c r="L64" s="23"/>
     </row>
-    <row r="65" spans="1:12" hidden="1">
+    <row r="65" spans="1:12">
       <c r="A65" s="19">
         <v>42937</v>
       </c>
@@ -10906,7 +10905,7 @@
       <c r="K65" s="23"/>
       <c r="L65" s="23"/>
     </row>
-    <row r="66" spans="1:12" hidden="1">
+    <row r="66" spans="1:12">
       <c r="A66" s="19">
         <v>42937</v>
       </c>
@@ -10937,7 +10936,7 @@
       <c r="K66" s="23"/>
       <c r="L66" s="23"/>
     </row>
-    <row r="67" spans="1:12" hidden="1">
+    <row r="67" spans="1:12">
       <c r="A67" s="19">
         <v>42937</v>
       </c>
@@ -10968,7 +10967,7 @@
       <c r="K67" s="23"/>
       <c r="L67" s="23"/>
     </row>
-    <row r="68" spans="1:12" hidden="1">
+    <row r="68" spans="1:12">
       <c r="A68" s="19">
         <v>42937</v>
       </c>
@@ -10999,7 +10998,7 @@
       <c r="K68" s="23"/>
       <c r="L68" s="23"/>
     </row>
-    <row r="69" spans="1:12" hidden="1">
+    <row r="69" spans="1:12">
       <c r="A69" s="19">
         <v>42937</v>
       </c>
@@ -11030,7 +11029,7 @@
       <c r="K69" s="23"/>
       <c r="L69" s="23"/>
     </row>
-    <row r="70" spans="1:12" hidden="1">
+    <row r="70" spans="1:12">
       <c r="A70" s="19">
         <v>42937</v>
       </c>
@@ -11061,7 +11060,7 @@
       <c r="K70" s="23"/>
       <c r="L70" s="23"/>
     </row>
-    <row r="71" spans="1:12" hidden="1">
+    <row r="71" spans="1:12">
       <c r="A71" s="19">
         <v>42937</v>
       </c>
@@ -11092,7 +11091,7 @@
       <c r="K71" s="23"/>
       <c r="L71" s="23"/>
     </row>
-    <row r="72" spans="1:12" hidden="1">
+    <row r="72" spans="1:12">
       <c r="A72" s="19">
         <v>42937</v>
       </c>
@@ -11123,7 +11122,7 @@
       <c r="K72" s="23"/>
       <c r="L72" s="23"/>
     </row>
-    <row r="73" spans="1:12" hidden="1">
+    <row r="73" spans="1:12">
       <c r="A73" s="19">
         <v>42937</v>
       </c>
@@ -11154,7 +11153,7 @@
       <c r="K73" s="23"/>
       <c r="L73" s="23"/>
     </row>
-    <row r="74" spans="1:12" hidden="1">
+    <row r="74" spans="1:12">
       <c r="A74" s="19">
         <v>42937</v>
       </c>
@@ -11185,7 +11184,7 @@
       <c r="K74" s="23"/>
       <c r="L74" s="23"/>
     </row>
-    <row r="75" spans="1:12" hidden="1">
+    <row r="75" spans="1:12">
       <c r="A75" s="19">
         <v>42937</v>
       </c>
@@ -11216,7 +11215,7 @@
       <c r="K75" s="23"/>
       <c r="L75" s="23"/>
     </row>
-    <row r="76" spans="1:12" hidden="1">
+    <row r="76" spans="1:12">
       <c r="A76" s="19">
         <v>42937</v>
       </c>
@@ -11247,7 +11246,7 @@
       <c r="K76" s="23"/>
       <c r="L76" s="23"/>
     </row>
-    <row r="77" spans="1:12" hidden="1">
+    <row r="77" spans="1:12">
       <c r="A77" s="19">
         <v>42937</v>
       </c>
@@ -11278,7 +11277,7 @@
       <c r="K77" s="23"/>
       <c r="L77" s="23"/>
     </row>
-    <row r="78" spans="1:12" hidden="1">
+    <row r="78" spans="1:12">
       <c r="A78" s="19">
         <v>42937</v>
       </c>
@@ -11309,7 +11308,7 @@
       <c r="K78" s="23"/>
       <c r="L78" s="23"/>
     </row>
-    <row r="79" spans="1:12" hidden="1">
+    <row r="79" spans="1:12">
       <c r="A79" s="19">
         <v>42937</v>
       </c>
@@ -11340,7 +11339,7 @@
       <c r="K79" s="23"/>
       <c r="L79" s="23"/>
     </row>
-    <row r="80" spans="1:12" hidden="1">
+    <row r="80" spans="1:12">
       <c r="A80" s="19">
         <v>42937</v>
       </c>
@@ -11371,7 +11370,7 @@
       <c r="K80" s="23"/>
       <c r="L80" s="23"/>
     </row>
-    <row r="81" spans="1:13" hidden="1">
+    <row r="81" spans="1:13">
       <c r="A81" s="19">
         <v>42937</v>
       </c>
@@ -11402,7 +11401,7 @@
       <c r="K81" s="23"/>
       <c r="L81" s="23"/>
     </row>
-    <row r="82" spans="1:13" hidden="1">
+    <row r="82" spans="1:13">
       <c r="A82" s="19">
         <v>42937</v>
       </c>
@@ -11433,7 +11432,7 @@
       <c r="K82" s="23"/>
       <c r="L82" s="23"/>
     </row>
-    <row r="83" spans="1:13" hidden="1">
+    <row r="83" spans="1:13">
       <c r="A83" s="19">
         <v>42937</v>
       </c>
@@ -11464,7 +11463,7 @@
       <c r="K83" s="23"/>
       <c r="L83" s="23"/>
     </row>
-    <row r="84" spans="1:13" hidden="1">
+    <row r="84" spans="1:13">
       <c r="A84" s="19">
         <v>42937</v>
       </c>
@@ -11495,7 +11494,7 @@
       <c r="K84" s="23"/>
       <c r="L84" s="23"/>
     </row>
-    <row r="85" spans="1:13" hidden="1">
+    <row r="85" spans="1:13">
       <c r="A85" s="19">
         <v>42937</v>
       </c>
@@ -11526,7 +11525,7 @@
       <c r="K85" s="23"/>
       <c r="L85" s="23"/>
     </row>
-    <row r="86" spans="1:13" hidden="1">
+    <row r="86" spans="1:13">
       <c r="A86" s="19">
         <v>42937</v>
       </c>
@@ -11557,7 +11556,7 @@
       <c r="K86" s="23"/>
       <c r="L86" s="23"/>
     </row>
-    <row r="87" spans="1:13" hidden="1">
+    <row r="87" spans="1:13">
       <c r="A87" s="19">
         <v>42937</v>
       </c>
@@ -11588,7 +11587,7 @@
       <c r="K87" s="23"/>
       <c r="L87" s="23"/>
     </row>
-    <row r="88" spans="1:13" hidden="1">
+    <row r="88" spans="1:13">
       <c r="A88" s="19">
         <v>42937</v>
       </c>
@@ -11619,7 +11618,7 @@
       <c r="K88" s="23"/>
       <c r="L88" s="23"/>
     </row>
-    <row r="89" spans="1:13" hidden="1">
+    <row r="89" spans="1:13">
       <c r="A89" s="19">
         <v>42937</v>
       </c>
@@ -11650,7 +11649,7 @@
       <c r="K89" s="23"/>
       <c r="L89" s="23"/>
     </row>
-    <row r="90" spans="1:13" hidden="1">
+    <row r="90" spans="1:13">
       <c r="A90" s="19">
         <v>42937</v>
       </c>
@@ -11681,7 +11680,7 @@
       <c r="K90" s="23"/>
       <c r="L90" s="23"/>
     </row>
-    <row r="91" spans="1:13" hidden="1">
+    <row r="91" spans="1:13">
       <c r="A91" s="19">
         <v>42937</v>
       </c>
@@ -11712,7 +11711,7 @@
       <c r="K91" s="23"/>
       <c r="L91" s="23"/>
     </row>
-    <row r="92" spans="1:13" hidden="1">
+    <row r="92" spans="1:13">
       <c r="A92" s="19">
         <v>42937</v>
       </c>
@@ -11743,7 +11742,7 @@
       <c r="K92" s="23"/>
       <c r="L92" s="23"/>
     </row>
-    <row r="93" spans="1:13" hidden="1">
+    <row r="93" spans="1:13">
       <c r="A93" s="19">
         <v>42937</v>
       </c>
@@ -11816,7 +11815,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1">
+    <row r="95" spans="1:13">
       <c r="A95" s="19">
         <v>42937</v>
       </c>
@@ -11847,7 +11846,7 @@
       <c r="K95" s="23"/>
       <c r="L95" s="23"/>
     </row>
-    <row r="96" spans="1:13" hidden="1">
+    <row r="96" spans="1:13">
       <c r="A96" s="19">
         <v>42937</v>
       </c>
@@ -11878,7 +11877,7 @@
       <c r="K96" s="23"/>
       <c r="L96" s="23"/>
     </row>
-    <row r="97" spans="1:13" hidden="1">
+    <row r="97" spans="1:13">
       <c r="A97" s="19">
         <v>42937</v>
       </c>
@@ -11909,7 +11908,7 @@
       <c r="K97" s="23"/>
       <c r="L97" s="23"/>
     </row>
-    <row r="98" spans="1:13" hidden="1">
+    <row r="98" spans="1:13">
       <c r="A98" s="19">
         <v>42937</v>
       </c>
@@ -11940,7 +11939,7 @@
       <c r="K98" s="23"/>
       <c r="L98" s="23"/>
     </row>
-    <row r="99" spans="1:13" hidden="1">
+    <row r="99" spans="1:13">
       <c r="A99" s="19">
         <v>42937</v>
       </c>
@@ -11971,7 +11970,7 @@
       <c r="K99" s="23"/>
       <c r="L99" s="23"/>
     </row>
-    <row r="100" spans="1:13" hidden="1">
+    <row r="100" spans="1:13">
       <c r="A100" s="19">
         <v>42937</v>
       </c>
@@ -12002,7 +12001,7 @@
       <c r="K100" s="23"/>
       <c r="L100" s="23"/>
     </row>
-    <row r="101" spans="1:13" hidden="1">
+    <row r="101" spans="1:13">
       <c r="A101" s="19">
         <v>42937</v>
       </c>
@@ -12033,7 +12032,7 @@
       <c r="K101" s="23"/>
       <c r="L101" s="23"/>
     </row>
-    <row r="102" spans="1:13" hidden="1">
+    <row r="102" spans="1:13">
       <c r="A102" s="19">
         <v>42937</v>
       </c>
@@ -12064,7 +12063,7 @@
       <c r="K102" s="23"/>
       <c r="L102" s="23"/>
     </row>
-    <row r="103" spans="1:13" hidden="1">
+    <row r="103" spans="1:13">
       <c r="A103" s="19">
         <v>42937</v>
       </c>
@@ -12095,7 +12094,7 @@
       <c r="K103" s="23"/>
       <c r="L103" s="23"/>
     </row>
-    <row r="104" spans="1:13" hidden="1">
+    <row r="104" spans="1:13">
       <c r="A104" s="19">
         <v>42937</v>
       </c>
@@ -12165,7 +12164,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="106" spans="1:13" hidden="1">
+    <row r="106" spans="1:13">
       <c r="A106" s="19">
         <v>42937</v>
       </c>
@@ -12195,7 +12194,7 @@
       <c r="K106" s="22"/>
       <c r="L106" s="23"/>
     </row>
-    <row r="107" spans="1:13" hidden="1">
+    <row r="107" spans="1:13">
       <c r="A107" s="19">
         <v>42937</v>
       </c>
@@ -12264,7 +12263,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1">
+    <row r="109" spans="1:13">
       <c r="A109" s="19">
         <v>42937</v>
       </c>
@@ -12295,7 +12294,7 @@
       <c r="K109" s="23"/>
       <c r="L109" s="23"/>
     </row>
-    <row r="110" spans="1:13" hidden="1">
+    <row r="110" spans="1:13">
       <c r="A110" s="19">
         <v>42937</v>
       </c>
@@ -12326,7 +12325,7 @@
       <c r="K110" s="23"/>
       <c r="L110" s="23"/>
     </row>
-    <row r="111" spans="1:13" hidden="1">
+    <row r="111" spans="1:13">
       <c r="A111" s="19">
         <v>42937</v>
       </c>
@@ -12357,7 +12356,7 @@
       <c r="K111" s="23"/>
       <c r="L111" s="23"/>
     </row>
-    <row r="112" spans="1:13" hidden="1">
+    <row r="112" spans="1:13">
       <c r="A112" s="19">
         <v>42937</v>
       </c>
@@ -12388,7 +12387,7 @@
       <c r="K112" s="23"/>
       <c r="L112" s="23"/>
     </row>
-    <row r="113" spans="1:13" hidden="1">
+    <row r="113" spans="1:13">
       <c r="A113" s="19">
         <v>42937</v>
       </c>
@@ -12453,7 +12452,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="115" spans="1:13" hidden="1">
+    <row r="115" spans="1:13">
       <c r="A115" s="19">
         <v>42937</v>
       </c>
@@ -12484,7 +12483,7 @@
       <c r="K115" s="23"/>
       <c r="L115" s="23"/>
     </row>
-    <row r="116" spans="1:13" hidden="1">
+    <row r="116" spans="1:13">
       <c r="A116" s="19">
         <v>42937</v>
       </c>
@@ -12515,7 +12514,7 @@
       <c r="K116" s="23"/>
       <c r="L116" s="23"/>
     </row>
-    <row r="117" spans="1:13" hidden="1">
+    <row r="117" spans="1:13">
       <c r="A117" s="19">
         <v>42937</v>
       </c>
@@ -12546,7 +12545,7 @@
       <c r="K117" s="23"/>
       <c r="L117" s="23"/>
     </row>
-    <row r="118" spans="1:13" hidden="1">
+    <row r="118" spans="1:13">
       <c r="A118" s="19">
         <v>42937</v>
       </c>
@@ -12574,7 +12573,7 @@
       <c r="K118" s="23"/>
       <c r="L118" s="23"/>
     </row>
-    <row r="119" spans="1:13" hidden="1">
+    <row r="119" spans="1:13">
       <c r="A119" s="19">
         <v>42937</v>
       </c>
@@ -12605,7 +12604,7 @@
       <c r="K119" s="23"/>
       <c r="L119" s="23"/>
     </row>
-    <row r="120" spans="1:13" hidden="1">
+    <row r="120" spans="1:13">
       <c r="A120" s="19">
         <v>42937</v>
       </c>
@@ -12675,7 +12674,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="122" spans="1:13" hidden="1">
+    <row r="122" spans="1:13">
       <c r="A122" s="19">
         <v>42937</v>
       </c>
@@ -12744,7 +12743,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1">
+    <row r="124" spans="1:13">
       <c r="A124" s="19">
         <v>42937</v>
       </c>
@@ -12774,7 +12773,7 @@
       <c r="K124" s="22"/>
       <c r="L124" s="23"/>
     </row>
-    <row r="125" spans="1:13" hidden="1">
+    <row r="125" spans="1:13">
       <c r="A125" s="19">
         <v>42937</v>
       </c>
@@ -12805,7 +12804,7 @@
       <c r="K125" s="23"/>
       <c r="L125" s="23"/>
     </row>
-    <row r="126" spans="1:13" hidden="1">
+    <row r="126" spans="1:13">
       <c r="A126" s="19">
         <v>42937</v>
       </c>
@@ -12836,7 +12835,7 @@
       <c r="K126" s="23"/>
       <c r="L126" s="23"/>
     </row>
-    <row r="127" spans="1:13" hidden="1">
+    <row r="127" spans="1:13">
       <c r="A127" s="19">
         <v>42937</v>
       </c>
@@ -12906,7 +12905,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1">
+    <row r="129" spans="1:13">
       <c r="A129" s="19">
         <v>42937</v>
       </c>
@@ -12975,7 +12974,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="131" spans="1:13" hidden="1">
+    <row r="131" spans="1:13">
       <c r="A131" s="19">
         <v>42937</v>
       </c>
@@ -13006,7 +13005,7 @@
       <c r="K131" s="23"/>
       <c r="L131" s="23"/>
     </row>
-    <row r="132" spans="1:13" hidden="1">
+    <row r="132" spans="1:13">
       <c r="A132" s="19">
         <v>42937</v>
       </c>
@@ -13037,7 +13036,7 @@
       <c r="K132" s="23"/>
       <c r="L132" s="23"/>
     </row>
-    <row r="133" spans="1:13" hidden="1">
+    <row r="133" spans="1:13">
       <c r="A133" s="19">
         <v>42937</v>
       </c>
@@ -13068,7 +13067,7 @@
       <c r="K133" s="23"/>
       <c r="L133" s="23"/>
     </row>
-    <row r="134" spans="1:13" hidden="1">
+    <row r="134" spans="1:13">
       <c r="A134" s="19">
         <v>42937</v>
       </c>
@@ -13099,7 +13098,7 @@
       <c r="K134" s="23"/>
       <c r="L134" s="23"/>
     </row>
-    <row r="135" spans="1:13" hidden="1">
+    <row r="135" spans="1:13">
       <c r="A135" s="19">
         <v>42937</v>
       </c>
@@ -13130,7 +13129,7 @@
       <c r="K135" s="23"/>
       <c r="L135" s="23"/>
     </row>
-    <row r="136" spans="1:13" hidden="1">
+    <row r="136" spans="1:13">
       <c r="A136" s="19">
         <v>42937</v>
       </c>
@@ -13161,7 +13160,7 @@
       <c r="K136" s="23"/>
       <c r="L136" s="23"/>
     </row>
-    <row r="137" spans="1:13" hidden="1">
+    <row r="137" spans="1:13">
       <c r="A137" s="19">
         <v>42937</v>
       </c>
@@ -13192,7 +13191,7 @@
       <c r="K137" s="23"/>
       <c r="L137" s="23"/>
     </row>
-    <row r="138" spans="1:13" hidden="1">
+    <row r="138" spans="1:13">
       <c r="A138" s="19">
         <v>42937</v>
       </c>
@@ -13262,7 +13261,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="140" spans="1:13" hidden="1">
+    <row r="140" spans="1:13">
       <c r="A140" s="19">
         <v>42937</v>
       </c>
@@ -13331,7 +13330,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="142" spans="1:13" hidden="1">
+    <row r="142" spans="1:13">
       <c r="A142" s="19">
         <v>42937</v>
       </c>
@@ -13400,7 +13399,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1">
+    <row r="144" spans="1:13">
       <c r="A144" s="19">
         <v>42937</v>
       </c>
@@ -13431,7 +13430,7 @@
       <c r="K144" s="23"/>
       <c r="L144" s="23"/>
     </row>
-    <row r="145" spans="1:13" hidden="1">
+    <row r="145" spans="1:13">
       <c r="A145" s="19">
         <v>42937</v>
       </c>
@@ -13462,7 +13461,7 @@
       <c r="K145" s="23"/>
       <c r="L145" s="23"/>
     </row>
-    <row r="146" spans="1:13" hidden="1">
+    <row r="146" spans="1:13">
       <c r="A146" s="19">
         <v>42937</v>
       </c>
@@ -13493,7 +13492,7 @@
       <c r="K146" s="23"/>
       <c r="L146" s="23"/>
     </row>
-    <row r="147" spans="1:13" hidden="1">
+    <row r="147" spans="1:13">
       <c r="A147" s="19">
         <v>42937</v>
       </c>
@@ -13524,7 +13523,7 @@
       <c r="K147" s="23"/>
       <c r="L147" s="23"/>
     </row>
-    <row r="148" spans="1:13" hidden="1">
+    <row r="148" spans="1:13">
       <c r="A148" s="19">
         <v>42937</v>
       </c>
@@ -13555,7 +13554,7 @@
       <c r="K148" s="23"/>
       <c r="L148" s="23"/>
     </row>
-    <row r="149" spans="1:13" hidden="1">
+    <row r="149" spans="1:13">
       <c r="A149" s="19">
         <v>42937</v>
       </c>
@@ -13586,7 +13585,7 @@
       <c r="K149" s="23"/>
       <c r="L149" s="23"/>
     </row>
-    <row r="150" spans="1:13" hidden="1">
+    <row r="150" spans="1:13">
       <c r="A150" s="19">
         <v>42937</v>
       </c>
@@ -13656,7 +13655,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="152" spans="1:13" hidden="1">
+    <row r="152" spans="1:13">
       <c r="A152" s="19">
         <v>42937</v>
       </c>
@@ -13725,7 +13724,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="154" spans="1:13" hidden="1">
+    <row r="154" spans="1:13">
       <c r="A154" s="19">
         <v>42937</v>
       </c>
@@ -13756,7 +13755,7 @@
       <c r="K154" s="23"/>
       <c r="L154" s="23"/>
     </row>
-    <row r="155" spans="1:13" hidden="1">
+    <row r="155" spans="1:13">
       <c r="A155" s="19">
         <v>42937</v>
       </c>
@@ -13821,7 +13820,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="157" spans="1:13" hidden="1">
+    <row r="157" spans="1:13">
       <c r="A157" s="19">
         <v>42937</v>
       </c>
@@ -13852,7 +13851,7 @@
       <c r="K157" s="23"/>
       <c r="L157" s="23"/>
     </row>
-    <row r="158" spans="1:13" hidden="1">
+    <row r="158" spans="1:13">
       <c r="A158" s="19">
         <v>42937</v>
       </c>
@@ -13883,7 +13882,7 @@
       <c r="K158" s="23"/>
       <c r="L158" s="23"/>
     </row>
-    <row r="159" spans="1:13" hidden="1">
+    <row r="159" spans="1:13">
       <c r="A159" s="19">
         <v>42937</v>
       </c>
@@ -13916,7 +13915,7 @@
       <c r="K159" s="23"/>
       <c r="L159" s="23"/>
     </row>
-    <row r="160" spans="1:13" hidden="1">
+    <row r="160" spans="1:13">
       <c r="A160" s="19">
         <v>42937</v>
       </c>
@@ -13947,7 +13946,7 @@
       <c r="K160" s="23"/>
       <c r="L160" s="23"/>
     </row>
-    <row r="161" spans="1:13" hidden="1">
+    <row r="161" spans="1:13">
       <c r="A161" s="19">
         <v>42937</v>
       </c>
@@ -13978,7 +13977,7 @@
       <c r="K161" s="23"/>
       <c r="L161" s="23"/>
     </row>
-    <row r="162" spans="1:13" hidden="1">
+    <row r="162" spans="1:13">
       <c r="A162" s="19">
         <v>42937</v>
       </c>
@@ -14009,7 +14008,7 @@
       <c r="K162" s="23"/>
       <c r="L162" s="23"/>
     </row>
-    <row r="163" spans="1:13" hidden="1">
+    <row r="163" spans="1:13">
       <c r="A163" s="19">
         <v>42937</v>
       </c>
@@ -14040,7 +14039,7 @@
       <c r="K163" s="23"/>
       <c r="L163" s="23"/>
     </row>
-    <row r="164" spans="1:13" hidden="1">
+    <row r="164" spans="1:13">
       <c r="A164" s="19">
         <v>42937</v>
       </c>
@@ -14071,7 +14070,7 @@
       <c r="K164" s="23"/>
       <c r="L164" s="23"/>
     </row>
-    <row r="165" spans="1:13" hidden="1">
+    <row r="165" spans="1:13">
       <c r="A165" s="19">
         <v>42937</v>
       </c>
@@ -14141,7 +14140,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="167" spans="1:13" hidden="1">
+    <row r="167" spans="1:13">
       <c r="A167" s="19">
         <v>42937</v>
       </c>
@@ -14210,7 +14209,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="169" spans="1:13" hidden="1">
+    <row r="169" spans="1:13">
       <c r="A169" s="19">
         <v>42937</v>
       </c>
@@ -14240,7 +14239,7 @@
       <c r="K169" s="22"/>
       <c r="L169" s="23"/>
     </row>
-    <row r="170" spans="1:13" hidden="1">
+    <row r="170" spans="1:13">
       <c r="A170" s="19">
         <v>42937</v>
       </c>
@@ -14309,7 +14308,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="172" spans="1:13" hidden="1">
+    <row r="172" spans="1:13">
       <c r="A172" s="19">
         <v>42937</v>
       </c>
@@ -14378,7 +14377,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="174" spans="1:13" hidden="1">
+    <row r="174" spans="1:13">
       <c r="A174" s="19">
         <v>42937</v>
       </c>
@@ -14408,7 +14407,7 @@
       <c r="K174" s="22"/>
       <c r="L174" s="23"/>
     </row>
-    <row r="175" spans="1:13" hidden="1">
+    <row r="175" spans="1:13">
       <c r="A175" s="19">
         <v>42937</v>
       </c>
@@ -14477,7 +14476,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="177" spans="1:13" hidden="1">
+    <row r="177" spans="1:13">
       <c r="A177" s="19">
         <v>42937</v>
       </c>
@@ -14546,7 +14545,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="179" spans="1:13" hidden="1">
+    <row r="179" spans="1:13">
       <c r="A179" s="19">
         <v>42937</v>
       </c>
@@ -14615,7 +14614,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="181" spans="1:13" hidden="1">
+    <row r="181" spans="1:13">
       <c r="A181" s="19">
         <v>42937</v>
       </c>
@@ -14646,7 +14645,7 @@
       <c r="K181" s="23"/>
       <c r="L181" s="23"/>
     </row>
-    <row r="182" spans="1:13" hidden="1">
+    <row r="182" spans="1:13">
       <c r="A182" s="19">
         <v>42937</v>
       </c>
@@ -14677,7 +14676,7 @@
       <c r="K182" s="23"/>
       <c r="L182" s="23"/>
     </row>
-    <row r="183" spans="1:13" hidden="1">
+    <row r="183" spans="1:13">
       <c r="A183" s="19">
         <v>42937</v>
       </c>
@@ -14710,7 +14709,7 @@
       <c r="K183" s="23"/>
       <c r="L183" s="23"/>
     </row>
-    <row r="184" spans="1:13" hidden="1">
+    <row r="184" spans="1:13">
       <c r="A184" s="19">
         <v>42937</v>
       </c>
@@ -14780,7 +14779,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1">
+    <row r="186" spans="1:13">
       <c r="A186" s="19">
         <v>42937</v>
       </c>
@@ -14849,7 +14848,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="188" spans="1:13" hidden="1">
+    <row r="188" spans="1:13">
       <c r="A188" s="19">
         <v>42937</v>
       </c>
@@ -14918,7 +14917,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="190" spans="1:13" hidden="1">
+    <row r="190" spans="1:13">
       <c r="A190" s="19">
         <v>42937</v>
       </c>
@@ -14987,7 +14986,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="192" spans="1:13" hidden="1">
+    <row r="192" spans="1:13">
       <c r="A192" s="19">
         <v>42937</v>
       </c>
@@ -15018,7 +15017,7 @@
       <c r="K192" s="23"/>
       <c r="L192" s="23"/>
     </row>
-    <row r="193" spans="1:13" hidden="1">
+    <row r="193" spans="1:13">
       <c r="A193" s="19">
         <v>42937</v>
       </c>
@@ -15089,7 +15088,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="195" spans="1:13" hidden="1">
+    <row r="195" spans="1:13">
       <c r="A195" s="19">
         <v>42937</v>
       </c>
@@ -15160,7 +15159,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="197" spans="1:13" hidden="1">
+    <row r="197" spans="1:13">
       <c r="A197" s="19">
         <v>42937</v>
       </c>
@@ -15191,7 +15190,7 @@
       <c r="K197" s="23"/>
       <c r="L197" s="23"/>
     </row>
-    <row r="198" spans="1:13" hidden="1">
+    <row r="198" spans="1:13">
       <c r="A198" s="19">
         <v>42937</v>
       </c>
@@ -15261,7 +15260,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="200" spans="1:13" hidden="1">
+    <row r="200" spans="1:13">
       <c r="A200" s="19">
         <v>42937</v>
       </c>
@@ -15330,7 +15329,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="202" spans="1:13" hidden="1">
+    <row r="202" spans="1:13">
       <c r="A202" s="19">
         <v>42937</v>
       </c>
@@ -15361,7 +15360,7 @@
       <c r="K202" s="23"/>
       <c r="L202" s="23"/>
     </row>
-    <row r="203" spans="1:13" hidden="1">
+    <row r="203" spans="1:13">
       <c r="A203" s="19">
         <v>42937</v>
       </c>
@@ -15392,7 +15391,7 @@
       <c r="K203" s="23"/>
       <c r="L203" s="23"/>
     </row>
-    <row r="204" spans="1:13" hidden="1">
+    <row r="204" spans="1:13">
       <c r="A204" s="19">
         <v>42937</v>
       </c>
@@ -15423,7 +15422,7 @@
       <c r="K204" s="23"/>
       <c r="L204" s="23"/>
     </row>
-    <row r="205" spans="1:13" hidden="1">
+    <row r="205" spans="1:13">
       <c r="A205" s="19">
         <v>42937</v>
       </c>
@@ -15454,7 +15453,7 @@
       <c r="K205" s="23"/>
       <c r="L205" s="23"/>
     </row>
-    <row r="206" spans="1:13" hidden="1">
+    <row r="206" spans="1:13">
       <c r="A206" s="19">
         <v>42937</v>
       </c>
@@ -15485,7 +15484,7 @@
       <c r="K206" s="23"/>
       <c r="L206" s="23"/>
     </row>
-    <row r="207" spans="1:13" hidden="1">
+    <row r="207" spans="1:13">
       <c r="A207" s="19">
         <v>42937</v>
       </c>
@@ -15556,7 +15555,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="209" spans="1:13" hidden="1">
+    <row r="209" spans="1:13">
       <c r="A209" s="19">
         <v>42937</v>
       </c>
@@ -15587,7 +15586,7 @@
       <c r="K209" s="23"/>
       <c r="L209" s="23"/>
     </row>
-    <row r="210" spans="1:13" hidden="1">
+    <row r="210" spans="1:13">
       <c r="A210" s="19">
         <v>42937</v>
       </c>
@@ -15693,7 +15692,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="213" spans="1:13" hidden="1">
+    <row r="213" spans="1:13">
       <c r="A213" s="19">
         <v>42937</v>
       </c>
@@ -15721,7 +15720,7 @@
       </c>
       <c r="J213" s="28"/>
     </row>
-    <row r="214" spans="1:13" hidden="1">
+    <row r="214" spans="1:13">
       <c r="A214" s="19">
         <v>42937</v>
       </c>
@@ -15749,7 +15748,7 @@
       </c>
       <c r="J214" s="28"/>
     </row>
-    <row r="215" spans="1:13" hidden="1">
+    <row r="215" spans="1:13">
       <c r="A215" s="19">
         <v>42937</v>
       </c>
@@ -15816,7 +15815,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="217" spans="1:13" hidden="1">
+    <row r="217" spans="1:13">
       <c r="A217" s="19">
         <v>42937</v>
       </c>
@@ -15883,7 +15882,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="219" spans="1:13" hidden="1">
+    <row r="219" spans="1:13">
       <c r="A219" s="19">
         <v>42937</v>
       </c>
@@ -15950,7 +15949,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="221" spans="1:13" hidden="1">
+    <row r="221" spans="1:13">
       <c r="A221" s="19">
         <v>42937</v>
       </c>
@@ -16056,7 +16055,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="224" spans="1:13" hidden="1">
+    <row r="224" spans="1:13">
       <c r="A224" s="19">
         <v>42937</v>
       </c>
@@ -16123,7 +16122,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="226" spans="1:13" hidden="1">
+    <row r="226" spans="1:13">
       <c r="A226" s="19">
         <v>42937</v>
       </c>
@@ -16190,7 +16189,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="228" spans="1:13" hidden="1">
+    <row r="228" spans="1:13">
       <c r="A228" s="19">
         <v>42937</v>
       </c>
@@ -16218,7 +16217,7 @@
       </c>
       <c r="J228" s="28"/>
     </row>
-    <row r="229" spans="1:13" hidden="1">
+    <row r="229" spans="1:13">
       <c r="A229" s="19">
         <v>42937</v>
       </c>
@@ -16285,7 +16284,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="231" spans="1:13" hidden="1">
+    <row r="231" spans="1:13">
       <c r="A231" s="19">
         <v>42937</v>
       </c>
@@ -16313,7 +16312,7 @@
       </c>
       <c r="J231" s="28"/>
     </row>
-    <row r="232" spans="1:13" hidden="1">
+    <row r="232" spans="1:13">
       <c r="A232" s="19">
         <v>42937</v>
       </c>
@@ -16341,7 +16340,7 @@
       </c>
       <c r="J232" s="28"/>
     </row>
-    <row r="233" spans="1:13" hidden="1">
+    <row r="233" spans="1:13">
       <c r="A233" s="19">
         <v>42937</v>
       </c>
@@ -16447,7 +16446,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="236" spans="1:13" hidden="1">
+    <row r="236" spans="1:13">
       <c r="A236" s="19">
         <v>42937</v>
       </c>
@@ -16475,7 +16474,7 @@
       </c>
       <c r="J236" s="28"/>
     </row>
-    <row r="237" spans="1:13" hidden="1">
+    <row r="237" spans="1:13">
       <c r="A237" s="19">
         <v>42937</v>
       </c>
@@ -16503,7 +16502,7 @@
       </c>
       <c r="J237" s="28"/>
     </row>
-    <row r="238" spans="1:13" hidden="1">
+    <row r="238" spans="1:13">
       <c r="A238" s="19">
         <v>42937</v>
       </c>
@@ -16570,7 +16569,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="240" spans="1:13" hidden="1">
+    <row r="240" spans="1:13">
       <c r="A240" s="19">
         <v>42937</v>
       </c>
@@ -16598,7 +16597,7 @@
       </c>
       <c r="J240" s="28"/>
     </row>
-    <row r="241" spans="1:13" hidden="1">
+    <row r="241" spans="1:13">
       <c r="A241" s="19">
         <v>42937</v>
       </c>
@@ -16704,7 +16703,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="244" spans="1:13" hidden="1">
+    <row r="244" spans="1:13">
       <c r="A244" s="19">
         <v>42937</v>
       </c>
@@ -16771,7 +16770,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="246" spans="1:13" hidden="1">
+    <row r="246" spans="1:13">
       <c r="A246" s="19">
         <v>42937</v>
       </c>
@@ -16799,7 +16798,7 @@
       </c>
       <c r="J246" s="28"/>
     </row>
-    <row r="247" spans="1:13" hidden="1">
+    <row r="247" spans="1:13">
       <c r="A247" s="19">
         <v>42937</v>
       </c>
@@ -16827,7 +16826,7 @@
       </c>
       <c r="J247" s="28"/>
     </row>
-    <row r="248" spans="1:13" hidden="1">
+    <row r="248" spans="1:13">
       <c r="A248" s="19">
         <v>42937</v>
       </c>
@@ -16894,7 +16893,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="250" spans="1:13" hidden="1">
+    <row r="250" spans="1:13">
       <c r="A250" s="19">
         <v>42937</v>
       </c>
@@ -16961,7 +16960,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="252" spans="1:13" hidden="1">
+    <row r="252" spans="1:13">
       <c r="A252" s="19">
         <v>42937</v>
       </c>
@@ -16989,7 +16988,7 @@
       </c>
       <c r="J252" s="28"/>
     </row>
-    <row r="253" spans="1:13" hidden="1">
+    <row r="253" spans="1:13">
       <c r="A253" s="19">
         <v>42937</v>
       </c>
@@ -17056,7 +17055,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="255" spans="1:13" hidden="1">
+    <row r="255" spans="1:13">
       <c r="A255" s="19">
         <v>42937</v>
       </c>
@@ -17084,7 +17083,7 @@
       </c>
       <c r="J255" s="28"/>
     </row>
-    <row r="256" spans="1:13" hidden="1">
+    <row r="256" spans="1:13">
       <c r="A256" s="19">
         <v>42937</v>
       </c>
@@ -17151,7 +17150,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="258" spans="1:13" hidden="1">
+    <row r="258" spans="1:13">
       <c r="A258" s="19">
         <v>42937</v>
       </c>
@@ -17179,7 +17178,7 @@
       </c>
       <c r="J258" s="28"/>
     </row>
-    <row r="259" spans="1:13" hidden="1">
+    <row r="259" spans="1:13">
       <c r="A259" s="19">
         <v>42937</v>
       </c>
@@ -17246,7 +17245,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="261" spans="1:13" hidden="1">
+    <row r="261" spans="1:13">
       <c r="A261" s="19">
         <v>42937</v>
       </c>
@@ -17313,7 +17312,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="263" spans="1:13" hidden="1">
+    <row r="263" spans="1:13">
       <c r="A263" s="19">
         <v>42937</v>
       </c>
@@ -17380,7 +17379,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="265" spans="1:13" hidden="1">
+    <row r="265" spans="1:13">
       <c r="A265" s="19">
         <v>42937</v>
       </c>
@@ -17408,7 +17407,7 @@
       </c>
       <c r="J265" s="28"/>
     </row>
-    <row r="266" spans="1:13" hidden="1">
+    <row r="266" spans="1:13">
       <c r="A266" s="19">
         <v>42937</v>
       </c>
@@ -17436,7 +17435,7 @@
       </c>
       <c r="J266" s="28"/>
     </row>
-    <row r="267" spans="1:13" hidden="1">
+    <row r="267" spans="1:13">
       <c r="A267" s="19">
         <v>42937</v>
       </c>
@@ -17503,7 +17502,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="269" spans="1:13" hidden="1">
+    <row r="269" spans="1:13">
       <c r="A269" s="19">
         <v>42937</v>
       </c>
@@ -17570,7 +17569,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="271" spans="1:13" hidden="1">
+    <row r="271" spans="1:13">
       <c r="A271" s="19">
         <v>42937</v>
       </c>
@@ -17637,7 +17636,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="273" spans="1:13" hidden="1">
+    <row r="273" spans="1:13">
       <c r="A273" s="19">
         <v>42937</v>
       </c>
@@ -17665,7 +17664,7 @@
       </c>
       <c r="J273" s="28"/>
     </row>
-    <row r="274" spans="1:13" hidden="1">
+    <row r="274" spans="1:13">
       <c r="A274" s="19">
         <v>42937</v>
       </c>
@@ -17732,7 +17731,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="276" spans="1:13" hidden="1">
+    <row r="276" spans="1:13">
       <c r="A276" s="19">
         <v>42937</v>
       </c>
@@ -17799,7 +17798,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="278" spans="1:13" hidden="1">
+    <row r="278" spans="1:13">
       <c r="A278" s="19">
         <v>42937</v>
       </c>
@@ -17866,7 +17865,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="280" spans="1:13" hidden="1">
+    <row r="280" spans="1:13">
       <c r="A280" s="19">
         <v>42937</v>
       </c>
@@ -17933,7 +17932,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="282" spans="1:13" hidden="1">
+    <row r="282" spans="1:13">
       <c r="A282" s="19">
         <v>42937</v>
       </c>
@@ -18000,7 +17999,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="284" spans="1:13" hidden="1">
+    <row r="284" spans="1:13">
       <c r="A284" s="19">
         <v>42937</v>
       </c>
@@ -18106,7 +18105,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="287" spans="1:13" hidden="1">
+    <row r="287" spans="1:13">
       <c r="A287" s="19">
         <v>42937</v>
       </c>
@@ -18134,7 +18133,7 @@
       </c>
       <c r="J287" s="28"/>
     </row>
-    <row r="288" spans="1:13" hidden="1">
+    <row r="288" spans="1:13">
       <c r="A288" s="19">
         <v>42937</v>
       </c>
@@ -18162,7 +18161,7 @@
       </c>
       <c r="J288" s="28"/>
     </row>
-    <row r="289" spans="1:13" hidden="1">
+    <row r="289" spans="1:13">
       <c r="A289" s="19">
         <v>42937</v>
       </c>
@@ -18186,7 +18185,7 @@
       </c>
       <c r="J289" s="28"/>
     </row>
-    <row r="290" spans="1:13" hidden="1">
+    <row r="290" spans="1:13">
       <c r="A290" s="19">
         <v>42937</v>
       </c>
@@ -18253,7 +18252,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="292" spans="1:13" hidden="1">
+    <row r="292" spans="1:13">
       <c r="A292" s="19">
         <v>42937</v>
       </c>
@@ -18281,7 +18280,7 @@
       </c>
       <c r="J292" s="28"/>
     </row>
-    <row r="293" spans="1:13" hidden="1">
+    <row r="293" spans="1:13">
       <c r="A293" s="19">
         <v>42937</v>
       </c>
@@ -18387,7 +18386,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="296" spans="1:13" hidden="1">
+    <row r="296" spans="1:13">
       <c r="A296" s="19">
         <v>42937</v>
       </c>
@@ -18493,7 +18492,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="299" spans="1:13" hidden="1">
+    <row r="299" spans="1:13">
       <c r="A299" s="19">
         <v>42937</v>
       </c>
@@ -18560,7 +18559,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="301" spans="1:13" hidden="1">
+    <row r="301" spans="1:13">
       <c r="A301" s="19">
         <v>42937</v>
       </c>
@@ -18627,7 +18626,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="303" spans="1:13" hidden="1">
+    <row r="303" spans="1:13">
       <c r="A303" s="19">
         <v>42937</v>
       </c>
@@ -18733,7 +18732,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="306" spans="1:13" hidden="1">
+    <row r="306" spans="1:13">
       <c r="A306" s="19">
         <v>42937</v>
       </c>
@@ -18800,7 +18799,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="308" spans="1:13" hidden="1">
+    <row r="308" spans="1:13">
       <c r="A308" s="19">
         <v>42937</v>
       </c>
@@ -18867,7 +18866,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="310" spans="1:13" hidden="1">
+    <row r="310" spans="1:13">
       <c r="A310" s="19">
         <v>42937</v>
       </c>
@@ -18934,7 +18933,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="312" spans="1:13" hidden="1">
+    <row r="312" spans="1:13">
       <c r="A312" s="19">
         <v>42937</v>
       </c>
@@ -19001,7 +19000,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="314" spans="1:13" hidden="1">
+    <row r="314" spans="1:13">
       <c r="A314" s="19">
         <v>42937</v>
       </c>
@@ -19068,7 +19067,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="316" spans="1:13" hidden="1">
+    <row r="316" spans="1:13">
       <c r="A316" s="19">
         <v>42937</v>
       </c>
@@ -19135,7 +19134,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="318" spans="1:13" hidden="1">
+    <row r="318" spans="1:13">
       <c r="A318" s="19">
         <v>42937</v>
       </c>
@@ -19202,7 +19201,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="320" spans="1:13" hidden="1">
+    <row r="320" spans="1:13">
       <c r="A320" s="19">
         <v>42937</v>
       </c>
@@ -19230,7 +19229,7 @@
       </c>
       <c r="J320" s="28"/>
     </row>
-    <row r="321" spans="1:13" hidden="1">
+    <row r="321" spans="1:13">
       <c r="A321" s="19">
         <v>42937</v>
       </c>
@@ -19258,7 +19257,7 @@
       </c>
       <c r="J321" s="28"/>
     </row>
-    <row r="322" spans="1:13" hidden="1">
+    <row r="322" spans="1:13">
       <c r="A322" s="19">
         <v>42937</v>
       </c>
@@ -19325,7 +19324,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="324" spans="1:13" hidden="1">
+    <row r="324" spans="1:13">
       <c r="A324" s="19">
         <v>42937</v>
       </c>
@@ -19392,7 +19391,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="326" spans="1:13" hidden="1">
+    <row r="326" spans="1:13">
       <c r="A326" s="19">
         <v>42937</v>
       </c>
@@ -19537,7 +19536,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="330" spans="1:13" hidden="1">
+    <row r="330" spans="1:13">
       <c r="A330" s="19">
         <v>42937</v>
       </c>
@@ -19604,7 +19603,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="332" spans="1:13" hidden="1">
+    <row r="332" spans="1:13">
       <c r="A332" s="19">
         <v>42937</v>
       </c>
@@ -19632,7 +19631,7 @@
       </c>
       <c r="J332" s="28"/>
     </row>
-    <row r="333" spans="1:13" hidden="1">
+    <row r="333" spans="1:13">
       <c r="A333" s="19">
         <v>42937</v>
       </c>
@@ -19660,7 +19659,7 @@
       </c>
       <c r="J333" s="28"/>
     </row>
-    <row r="334" spans="1:13" hidden="1">
+    <row r="334" spans="1:13">
       <c r="A334" s="19">
         <v>42937</v>
       </c>
@@ -19768,7 +19767,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="337" spans="1:13" hidden="1">
+    <row r="337" spans="1:13">
       <c r="A337" s="19">
         <v>42937</v>
       </c>
@@ -19796,7 +19795,7 @@
       </c>
       <c r="J337" s="28"/>
     </row>
-    <row r="338" spans="1:13" hidden="1">
+    <row r="338" spans="1:13">
       <c r="A338" s="19">
         <v>42937</v>
       </c>
@@ -19863,7 +19862,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="340" spans="1:13" hidden="1">
+    <row r="340" spans="1:13">
       <c r="A340" s="19">
         <v>42937</v>
       </c>
@@ -19891,7 +19890,7 @@
       </c>
       <c r="J340" s="28"/>
     </row>
-    <row r="341" spans="1:13" hidden="1">
+    <row r="341" spans="1:13">
       <c r="A341" s="19">
         <v>42937</v>
       </c>
@@ -19919,7 +19918,7 @@
       </c>
       <c r="J341" s="28"/>
     </row>
-    <row r="342" spans="1:13" hidden="1">
+    <row r="342" spans="1:13">
       <c r="A342" s="19">
         <v>42937</v>
       </c>
@@ -19947,7 +19946,7 @@
       </c>
       <c r="J342" s="28"/>
     </row>
-    <row r="343" spans="1:13" hidden="1">
+    <row r="343" spans="1:13">
       <c r="A343" s="19">
         <v>42937</v>
       </c>
@@ -19975,7 +19974,7 @@
       </c>
       <c r="J343" s="28"/>
     </row>
-    <row r="344" spans="1:13" hidden="1">
+    <row r="344" spans="1:13">
       <c r="A344" s="19">
         <v>42937</v>
       </c>
@@ -20003,7 +20002,7 @@
       </c>
       <c r="J344" s="28"/>
     </row>
-    <row r="345" spans="1:13" hidden="1">
+    <row r="345" spans="1:13">
       <c r="A345" s="19">
         <v>42937</v>
       </c>
@@ -20031,7 +20030,7 @@
       </c>
       <c r="J345" s="28"/>
     </row>
-    <row r="346" spans="1:13" hidden="1">
+    <row r="346" spans="1:13">
       <c r="A346" s="19">
         <v>42937</v>
       </c>
@@ -20137,7 +20136,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="349" spans="1:13" hidden="1">
+    <row r="349" spans="1:13">
       <c r="A349" s="19">
         <v>42937</v>
       </c>
@@ -20243,7 +20242,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="352" spans="1:13" hidden="1">
+    <row r="352" spans="1:13">
       <c r="A352" s="19">
         <v>42937</v>
       </c>
@@ -20310,7 +20309,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="354" spans="1:13" hidden="1">
+    <row r="354" spans="1:13">
       <c r="A354" s="19">
         <v>42937</v>
       </c>
@@ -20338,7 +20337,7 @@
       </c>
       <c r="J354" s="28"/>
     </row>
-    <row r="355" spans="1:13" hidden="1">
+    <row r="355" spans="1:13">
       <c r="A355" s="19">
         <v>42937</v>
       </c>
@@ -20405,7 +20404,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="357" spans="1:13" hidden="1">
+    <row r="357" spans="1:13">
       <c r="A357" s="19">
         <v>42937</v>
       </c>
@@ -20472,7 +20471,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="359" spans="1:13" hidden="1">
+    <row r="359" spans="1:13">
       <c r="A359" s="19">
         <v>42937</v>
       </c>
@@ -20539,7 +20538,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="361" spans="1:13" hidden="1">
+    <row r="361" spans="1:13">
       <c r="A361" s="19">
         <v>42937</v>
       </c>
@@ -20606,7 +20605,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="363" spans="1:13" hidden="1">
+    <row r="363" spans="1:13">
       <c r="A363" s="19">
         <v>42937</v>
       </c>
@@ -20673,7 +20672,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="365" spans="1:13" hidden="1">
+    <row r="365" spans="1:13">
       <c r="A365" s="19">
         <v>42937</v>
       </c>
@@ -20740,7 +20739,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="367" spans="1:13" hidden="1">
+    <row r="367" spans="1:13">
       <c r="A367" s="19">
         <v>42937</v>
       </c>
@@ -20807,7 +20806,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="369" spans="1:13" hidden="1">
+    <row r="369" spans="1:13">
       <c r="A369" s="19">
         <v>42937</v>
       </c>
@@ -20829,20 +20828,14 @@
       <c r="J369" s="28"/>
       <c r="M369" s="26"/>
     </row>
-    <row r="370" spans="1:13" hidden="1">
+    <row r="370" spans="1:13">
       <c r="G370">
         <f>SUM(G2:G369)</f>
         <v>10000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T370" xr:uid="{93D26894-34B3-49C7-AEF6-CD43A34AA7ED}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="HC"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:T370" xr:uid="{93D26894-34B3-49C7-AEF6-CD43A34AA7ED}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>